<commit_message>
endpoint para pegar subprefeitura do imovel
</commit_message>
<xml_diff>
--- a/data/codigos_zoneamento_SMDU.xlsx
+++ b/data/codigos_zoneamento_SMDU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d835916\Desktop\SISTEMAS\geoBdt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27075CD4-24BF-46D2-B99A-CBC9D0145CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E91E7F8-15C0-4C02-8C6F-6475810B47F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{23D04053-BEC1-4936-8786-5BD6814DFD6D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{23D04053-BEC1-4936-8786-5BD6814DFD6D}"/>
   </bookViews>
   <sheets>
     <sheet name="codigos_zoneamento" sheetId="1" r:id="rId1"/>
@@ -1809,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A245E37F-69E1-4122-B5C5-F3DE716B1D01}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42963C1-76AE-4C62-89BE-1B88C86C1D8C}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>